<commit_message>
Added a tables directory with useful tables and data for analysis
</commit_message>
<xml_diff>
--- a/tables/cable_response/coax_info.xlsx
+++ b/tables/cable_response/coax_info.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\blr\Dropbox (MIT)\MIT\Research\Projects\ptof_analysis\tables\cable_response\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{35F2F1EB-2D34-4EDC-A7EF-3C5B87EA0FB5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4BB9743B-E88A-43F0-AF52-BC57BC70E113}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="130" windowWidth="9640" windowHeight="8170" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="2280" yWindow="2280" windowWidth="14400" windowHeight="8170" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="13">
   <si>
     <t>cable type</t>
   </si>
@@ -70,6 +70,9 @@
   </si>
   <si>
     <t>g_c (S*m)</t>
+  </si>
+  <si>
+    <t>losstan</t>
   </si>
 </sst>
 </file>
@@ -388,10 +391,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:H7"/>
+  <dimension ref="A1:I7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D14" sqref="D14"/>
+      <selection activeCell="I5" sqref="I5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -401,7 +404,7 @@
     <col min="8" max="8" width="13.26953125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -426,8 +429,11 @@
       <c r="H1" t="s">
         <v>11</v>
       </c>
+      <c r="I1" t="s">
+        <v>12</v>
+      </c>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>2</v>
       </c>
@@ -455,8 +461,11 @@
       <c r="H2" s="1">
         <v>63000000</v>
       </c>
+      <c r="I2" s="1">
+        <v>6.9999999999999994E-5</v>
+      </c>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>5</v>
       </c>
@@ -484,8 +493,11 @@
       <c r="H3" s="1">
         <v>59600000</v>
       </c>
+      <c r="I3" s="1">
+        <v>2.9999999999999997E-4</v>
+      </c>
     </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
         <v>6</v>
       </c>
@@ -513,8 +525,11 @@
       <c r="H4" s="1">
         <v>59600000</v>
       </c>
+      <c r="I4" s="1">
+        <v>2.0000000000000001E-4</v>
+      </c>
     </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
         <v>7</v>
       </c>
@@ -542,8 +557,11 @@
       <c r="H5" s="1">
         <v>63000000</v>
       </c>
+      <c r="I5" s="1">
+        <v>6.9999999999999994E-5</v>
+      </c>
     </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:9" x14ac:dyDescent="0.35">
       <c r="F7" s="1"/>
     </row>
   </sheetData>

</xml_diff>